<commit_message>
mise à jour target et diagnose
</commit_message>
<xml_diff>
--- a/work/Centres_geo.xlsx
+++ b/work/Centres_geo.xlsx
@@ -4675,7 +4675,7 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
-    <col min="2" max="2" width="20" customWidth="1"/>
+    <col min="2" max="2" width="21" customWidth="1"/>
     <col min="3" max="3" width="29" customWidth="1"/>
     <col min="4" max="4" width="8" customWidth="1"/>
     <col min="5" max="5" width="13" customWidth="1"/>
@@ -5131,7 +5131,7 @@
         <v>47.398410522</v>
       </c>
       <c r="K11">
-        <v>0.6961002820000001</v>
+        <v>0.6961002820000002</v>
       </c>
       <c r="L11" t="s">
         <v>71</v>
@@ -5664,7 +5664,7 @@
         <v>44.857621613</v>
       </c>
       <c r="K24">
-        <v>-0.5733793060000001</v>
+        <v>-0.5733793060000002</v>
       </c>
       <c r="L24" t="s">
         <v>126</v>
@@ -6361,7 +6361,7 @@
         <v>47.398410522</v>
       </c>
       <c r="K41">
-        <v>0.6961002820000001</v>
+        <v>0.6961002820000002</v>
       </c>
       <c r="L41" t="s">
         <v>71</v>
@@ -8206,7 +8206,7 @@
         <v>47.398410522</v>
       </c>
       <c r="K86">
-        <v>0.6961002820000001</v>
+        <v>0.6961002820000002</v>
       </c>
       <c r="L86" t="s">
         <v>71</v>
@@ -10010,7 +10010,7 @@
         <v>47.398410522</v>
       </c>
       <c r="K130">
-        <v>0.6961002820000001</v>
+        <v>0.6961002820000002</v>
       </c>
       <c r="L130" t="s">
         <v>71</v>
@@ -10912,7 +10912,7 @@
         <v>44.202826475</v>
       </c>
       <c r="K152">
-        <v>0.6257305230000001</v>
+        <v>0.6257305230000002</v>
       </c>
       <c r="L152" t="s">
         <v>597</v>
@@ -11486,7 +11486,7 @@
         <v>44.202826475</v>
       </c>
       <c r="K166">
-        <v>0.6257305230000001</v>
+        <v>0.6257305230000002</v>
       </c>
       <c r="L166" t="s">
         <v>597</v>
@@ -11568,7 +11568,7 @@
         <v>44.202826475</v>
       </c>
       <c r="K168">
-        <v>0.6257305230000001</v>
+        <v>0.6257305230000002</v>
       </c>
       <c r="L168" t="s">
         <v>597</v>
@@ -11691,7 +11691,7 @@
         <v>44.857621613</v>
       </c>
       <c r="K171">
-        <v>-0.5733793060000001</v>
+        <v>-0.5733793060000002</v>
       </c>
       <c r="L171" t="s">
         <v>126</v>
@@ -12552,7 +12552,7 @@
         <v>44.857621613</v>
       </c>
       <c r="K192">
-        <v>-0.5733793060000001</v>
+        <v>-0.5733793060000002</v>
       </c>
       <c r="L192" t="s">
         <v>126</v>
@@ -13249,7 +13249,7 @@
         <v>44.857621613</v>
       </c>
       <c r="K209">
-        <v>-0.5733793060000001</v>
+        <v>-0.5733793060000002</v>
       </c>
       <c r="L209" t="s">
         <v>126</v>
@@ -14028,7 +14028,7 @@
         <v>47.398410522</v>
       </c>
       <c r="K228">
-        <v>0.6961002820000001</v>
+        <v>0.6961002820000002</v>
       </c>
       <c r="L228" t="s">
         <v>71</v>
@@ -14151,7 +14151,7 @@
         <v>47.398410522</v>
       </c>
       <c r="K231">
-        <v>0.6961002820000001</v>
+        <v>0.6961002820000002</v>
       </c>
       <c r="L231" t="s">
         <v>71</v>
@@ -14274,7 +14274,7 @@
         <v>47.398410522</v>
       </c>
       <c r="K234">
-        <v>0.6961002820000001</v>
+        <v>0.6961002820000002</v>
       </c>
       <c r="L234" t="s">
         <v>71</v>
@@ -14684,7 +14684,7 @@
         <v>44.857621613</v>
       </c>
       <c r="K244">
-        <v>-0.5733793060000001</v>
+        <v>-0.5733793060000002</v>
       </c>
       <c r="L244" t="s">
         <v>126</v>
@@ -17390,7 +17390,7 @@
         <v>44.202826475</v>
       </c>
       <c r="K310">
-        <v>0.6257305230000001</v>
+        <v>0.6257305230000002</v>
       </c>
       <c r="L310" t="s">
         <v>597</v>
@@ -17431,7 +17431,7 @@
         <v>47.398410522</v>
       </c>
       <c r="K311">
-        <v>0.6961002820000001</v>
+        <v>0.6961002820000002</v>
       </c>
       <c r="L311" t="s">
         <v>71</v>
@@ -19358,7 +19358,7 @@
         <v>47.398410522</v>
       </c>
       <c r="K358">
-        <v>0.6961002820000001</v>
+        <v>0.6961002820000002</v>
       </c>
       <c r="L358" t="s">
         <v>71</v>
@@ -19440,7 +19440,7 @@
         <v>47.398410522</v>
       </c>
       <c r="K360">
-        <v>0.6961002820000001</v>
+        <v>0.6961002820000002</v>
       </c>
       <c r="L360" t="s">
         <v>71</v>
@@ -21695,7 +21695,7 @@
         <v>44.857621613</v>
       </c>
       <c r="K415">
-        <v>-0.5733793060000001</v>
+        <v>-0.5733793060000002</v>
       </c>
       <c r="L415" t="s">
         <v>126</v>
@@ -21736,7 +21736,7 @@
         <v>44.857621613</v>
       </c>
       <c r="K416">
-        <v>-0.5733793060000001</v>
+        <v>-0.5733793060000002</v>
       </c>
       <c r="L416" t="s">
         <v>126</v>
@@ -21818,7 +21818,7 @@
         <v>44.202826475</v>
       </c>
       <c r="K418">
-        <v>0.6257305230000001</v>
+        <v>0.6257305230000002</v>
       </c>
       <c r="L418" t="s">
         <v>597</v>
@@ -24278,7 +24278,7 @@
         <v>44.857621613</v>
       </c>
       <c r="K478">
-        <v>-0.5733793060000001</v>
+        <v>-0.5733793060000002</v>
       </c>
       <c r="L478" t="s">
         <v>126</v>

</xml_diff>